<commit_message>
Working on evaluator outputs
</commit_message>
<xml_diff>
--- a/poi-generated-file.xlsx
+++ b/poi-generated-file.xlsx
@@ -17,9 +17,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="5">
-  <si>
-    <t>QRY NUMBER/Similaity Type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="17">
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Interpolated point/Similaity Type</t>
+  </si>
+  <si>
+    <t>Qry ID</t>
   </si>
   <si>
     <t>DICE</t>
@@ -76,34 +112,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.19140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.25390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.4921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.68359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.19140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.4921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -113,34 +203,93 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.19140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.25390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.4921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.68359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.19140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.4921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -150,34 +299,93 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.19140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.25390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.4921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.68359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.19140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.4921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -187,34 +395,93 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.19140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.25390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.4921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.68359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.19140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.4921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -224,34 +491,93 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.19140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.25390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.4921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.68359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.19140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.4921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -261,34 +587,93 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="26.69921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="5.19140625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="8.25390625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.4921875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.65625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.68359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="5.19140625" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.25390625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="11.671875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="21.4921875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>